<commit_message>
20230530 - completed DLAI-deeplearning specialization
</commit_message>
<xml_diff>
--- a/summary/20230503_certificates_MPS.xlsx
+++ b/summary/20230503_certificates_MPS.xlsx
@@ -8,8 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="20230502-Certificates" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Zusätzlich erworbene Zertifikat" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="WBS Bausteinprüfungen" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="82">
   <si>
     <t xml:space="preserve">Google data analytics professional certificate</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t xml:space="preserve">Ultimate Rust Crash Course</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/pstmps/Certificates</t>
   </si>
   <si>
     <t xml:space="preserve">WBS Bausteinpruefungen</t>
@@ -387,7 +390,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -430,6 +433,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -540,7 +547,7 @@
   <dimension ref="B3:F51"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D42" activeCellId="0" sqref="D42"/>
+      <selection pane="topLeft" activeCell="D36" activeCellId="0" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -549,7 +556,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="19.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="75.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="56.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="49.1"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -847,11 +855,10 @@
       <c r="F32" s="10"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="6"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="10"/>
+      <c r="B33" s="0"/>
+      <c r="C33" s="0"/>
+      <c r="D33" s="0"/>
+      <c r="F33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0"/>
@@ -868,7 +875,9 @@
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0"/>
       <c r="C36" s="0"/>
-      <c r="D36" s="0"/>
+      <c r="D36" s="11" t="s">
+        <v>35</v>
+      </c>
       <c r="F36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -968,10 +977,10 @@
     <mergeCell ref="B23:D23"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="0.954166666666667" bottom="0.7875" header="0.7875" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="71" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.528472222222222" right="0.491666666666667" top="1.54930555555556" bottom="0.7875" header="1.38263888888889" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="78" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;L&amp;"Times New Roman,Regular"&amp;12Michael-Philipp Stiebing&amp;R&amp;"Times New Roman,Regular"&amp;12m.stiebing@gmail.com</oddHeader>
+    <oddHeader>&amp;L&amp;"Times New Roman,Regular"&amp;12Michael-Philipp Stiebing&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A&amp;R&amp;"Times New Roman,Regular"&amp;12m.stiebing@gmail.com</oddHeader>
     <oddFooter/>
   </headerFooter>
 </worksheet>
@@ -985,11 +994,12 @@
   <dimension ref="B2:F19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D34" activeCellId="0" sqref="D34"/>
+      <selection pane="topLeft" activeCell="J47" activeCellId="0" sqref="J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="58.32"/>
@@ -997,19 +1007,19 @@
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="12" t="s">
+      <c r="E2" s="12" t="s">
         <v>37</v>
       </c>
+      <c r="F2" s="13" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="13"/>
+      <c r="B3" s="14"/>
       <c r="C3" s="7"/>
       <c r="D3" s="9"/>
       <c r="E3" s="7"/>
@@ -1017,210 +1027,210 @@
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="6"/>
       <c r="C4" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="15" t="n">
+      <c r="E4" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="16" t="n">
         <v>0.9658</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="6"/>
       <c r="C5" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="15" t="n">
+      <c r="E5" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="16" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="F6" s="15" t="n">
+      <c r="E6" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="16" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="6"/>
       <c r="C7" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="F7" s="15" t="n">
+      <c r="E7" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="16" t="n">
         <v>0.8851</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="6"/>
       <c r="C8" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="E8" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="15" t="n">
+      <c r="E8" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="16" t="n">
         <v>0.9286</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="6"/>
       <c r="C9" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E9" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="F9" s="15" t="n">
+      <c r="E9" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="16" t="n">
         <v>0.9686</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="6"/>
       <c r="C10" s="7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E10" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="F10" s="15" t="n">
+      <c r="E10" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="16" t="n">
         <v>0.8919</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="6"/>
       <c r="C11" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="E11" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="F11" s="15" t="n">
+      <c r="E11" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" s="16" t="n">
         <v>0.878</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="6"/>
       <c r="C12" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="E12" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="F12" s="15" t="n">
+      <c r="E12" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="16" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="6"/>
       <c r="C13" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="E13" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="F13" s="15" t="n">
+      <c r="E13" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="16" t="n">
         <v>0.9894</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="6"/>
       <c r="C14" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="E14" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="F14" s="15" t="n">
+      <c r="E14" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" s="16" t="n">
         <v>0.9268</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="6"/>
       <c r="C15" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="E15" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="F15" s="15" t="n">
+      <c r="E15" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F15" s="16" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="6"/>
       <c r="C16" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="E16" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="F16" s="15" t="n">
+      <c r="E16" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F16" s="16" t="n">
         <v>0.9556</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="6"/>
       <c r="C17" s="7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="E17" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="F17" s="15" t="n">
+      <c r="E17" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="F17" s="16" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1233,11 +1243,11 @@
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="6"/>
       <c r="C19" s="7"/>
-      <c r="D19" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="E19" s="16"/>
-      <c r="F19" s="17" t="n">
+      <c r="D19" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="E19" s="17"/>
+      <c r="F19" s="18" t="n">
         <f aca="false">AVERAGE(F4:F17)</f>
         <v>0.956414285714286</v>
       </c>
@@ -1247,11 +1257,13 @@
     <mergeCell ref="B2:D2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.7875" right="0.7875" top="2.25069444444444" bottom="0.886111111111111" header="1.98541666666667" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="78" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="true" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <firstHeader>&amp;L&amp;"Times New Roman,Regular"&amp;12Michael-Philipp Stiebing&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A&amp;R&amp;"Times New Roman,Regular"&amp;12m.stiebing@gmail.com</firstHeader>
+    <firstFooter/>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>